<commit_message>
Wireframes, arborescence et cas d'utilisation - Update
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Ajout des Wireframes.</t>
+  </si>
+  <si>
+    <t>Concernant SwissCenter, le dossier de projet et le journal de travail.</t>
   </si>
 </sst>
 </file>
@@ -674,7 +677,7 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,7 +1448,7 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" ref="E25:E31" si="3">D25-C25</f>
+        <f t="shared" ref="E25:E35" si="3">D25-C25</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -1652,8 +1655,13 @@
       <c r="C32" s="10">
         <v>0.40972222222222227</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="2"/>
+      <c r="D32" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="3"/>
+        <v>3.125E-2</v>
+      </c>
       <c r="F32" s="1" t="s">
         <v>23</v>
       </c>
@@ -1669,38 +1677,90 @@
       <c r="L32" s="21"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="2"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="20"/>
+      <c r="A33" s="8">
+        <v>44322</v>
+      </c>
+      <c r="B33" s="9">
+        <v>1</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0.46458333333333335</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0138888888888928E-2</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="I33" s="21"/>
       <c r="J33" s="21"/>
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="2"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
+    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>44322</v>
+      </c>
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
+      <c r="C34" s="10">
+        <v>0.46458333333333335</v>
+      </c>
+      <c r="D34" s="10">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="3"/>
+        <v>1.1111111111111072E-2</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="I34" s="21"/>
       <c r="J34" s="21"/>
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="2"/>
-      <c r="G35" s="19"/>
+      <c r="A35" s="8">
+        <v>44322</v>
+      </c>
+      <c r="B35" s="9">
+        <v>1</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="3"/>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="H35" s="20"/>
       <c r="I35" s="21"/>
       <c r="J35" s="21"/>
@@ -1708,12 +1768,23 @@
       <c r="L35" s="21"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
+      <c r="A36" s="8">
+        <v>44322</v>
+      </c>
+      <c r="B36" s="9">
+        <v>1</v>
+      </c>
+      <c r="C36" s="10">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="D36" s="10"/>
       <c r="E36" s="2"/>
-      <c r="G36" s="19"/>
+      <c r="F36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="H36" s="20"/>
       <c r="I36" s="21"/>
       <c r="J36" s="21"/>
@@ -2125,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Doc Étude de faisabilité
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Concernant SwissCenter, le dossier de projet et le journal de travail.</t>
+  </si>
+  <si>
+    <t>Rédaction de l'étude de faisabilité.</t>
   </si>
 </sst>
 </file>
@@ -676,8 +679,8 @@
   </sheetPr>
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,7 +1451,7 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" ref="E25:E35" si="3">D25-C25</f>
+        <f t="shared" ref="E25:E37" si="3">D25-C25</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -1775,10 +1778,15 @@
         <v>1</v>
       </c>
       <c r="C36" s="10">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="2"/>
+        <v>0.5625</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0.59375</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="3"/>
+        <v>3.125E-2</v>
+      </c>
       <c r="F36" s="1" t="s">
         <v>23</v>
       </c>
@@ -1792,13 +1800,31 @@
       <c r="L36" s="21"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="2"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="20"/>
+      <c r="A37" s="8">
+        <v>44322</v>
+      </c>
+      <c r="B37" s="9">
+        <v>1</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0.59375</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="3"/>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>50</v>
+      </c>
       <c r="I37" s="21"/>
       <c r="J37" s="21"/>
       <c r="K37" s="21"/>
@@ -1818,13 +1844,43 @@
       <c r="L38" s="21"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
       <c r="E39" s="2"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
       <c r="E40" s="2"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
       <c r="E41" s="2"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E42" s="2"/>

</xml_diff>

<commit_message>
Last doc update 06.05.21
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -160,19 +160,37 @@
     <t>Mail annonçant le changement du nombre de sprint précédemment cité.</t>
   </si>
   <si>
-    <t>Correction du diagramme d'arborescence du site.</t>
-  </si>
-  <si>
     <t>Diagramme: Arborescence du site: Utilisateur non authentifié, authentifié et administrateur.</t>
   </si>
   <si>
-    <t>Ajout des Wireframes.</t>
-  </si>
-  <si>
     <t>Concernant SwissCenter, le dossier de projet et le journal de travail.</t>
   </si>
   <si>
-    <t>Rédaction de l'étude de faisabilité.</t>
+    <t>Dossier de projet: Scénarios</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Étude de faisabilité.</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Ajout des Wireframes.</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Ajout et correction des Wireframes.</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Correction du diagramme d'arborescence du site.</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Correction des diagrammes de l'arborescence.</t>
+  </si>
+  <si>
+    <t>Réacquisition du sujet.</t>
+  </si>
+  <si>
+    <t>Manque d'informations sur le sujet.</t>
+  </si>
+  <si>
+    <t>Théorie sur la documentation: support_courtV3.5.2.pdf</t>
   </si>
 </sst>
 </file>
@@ -287,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -329,28 +347,152 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -679,8 +821,8 @@
   </sheetPr>
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,10 +834,7 @@
     <col min="5" max="5" width="7.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="30.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="40.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -723,16 +862,16 @@
       <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="19" t="s">
         <v>8</v>
       </c>
     </row>
@@ -762,12 +901,12 @@
       <c r="H2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>44319</v>
       </c>
@@ -787,16 +926,16 @@
       <c r="F3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
@@ -818,16 +957,16 @@
       <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+    </row>
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>44319</v>
       </c>
@@ -847,16 +986,16 @@
       <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -878,14 +1017,14 @@
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -907,14 +1046,14 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
@@ -936,14 +1075,14 @@
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -965,16 +1104,16 @@
       <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
@@ -996,18 +1135,18 @@
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>44319</v>
       </c>
@@ -1027,16 +1166,16 @@
       <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
@@ -1058,16 +1197,16 @@
       <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -1089,16 +1228,16 @@
       <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
@@ -1120,16 +1259,16 @@
       <c r="F14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1142,25 +1281,25 @@
         <v>0.69097222222222221</v>
       </c>
       <c r="D15" s="10">
-        <v>0.70138888888888884</v>
+        <v>0.70486111111111116</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>1.041666666666663E-2</v>
+        <v>1.3888888888888951E-2</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -1182,16 +1321,16 @@
       <c r="F16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1213,16 +1352,16 @@
       <c r="F17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
@@ -1244,16 +1383,16 @@
       <c r="F18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
@@ -1275,14 +1414,14 @@
       <c r="F19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
@@ -1304,16 +1443,16 @@
       <c r="F20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
@@ -1335,14 +1474,14 @@
       <c r="F21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
@@ -1364,16 +1503,16 @@
       <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H22" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
@@ -1395,16 +1534,16 @@
       <c r="F23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21" t="s">
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
@@ -1426,16 +1565,16 @@
       <c r="F24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
@@ -1451,22 +1590,22 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" ref="E25:E37" si="3">D25-C25</f>
+        <f t="shared" ref="E25:E38" si="3">D25-C25</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="H25" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
@@ -1488,14 +1627,14 @@
       <c r="F26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
@@ -1517,16 +1656,16 @@
       <c r="F27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H27" s="20"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+    </row>
+    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>44322</v>
       </c>
@@ -1546,18 +1685,18 @@
       <c r="F28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="G28" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-    </row>
-    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="H28" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+    </row>
+    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>44322</v>
       </c>
@@ -1577,16 +1716,16 @@
       <c r="F29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H29" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
+      <c r="H29" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
@@ -1608,14 +1747,14 @@
       <c r="F30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="G30" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H30" s="17"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
@@ -1637,16 +1776,16 @@
       <c r="F31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
+      <c r="H31" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
@@ -1668,18 +1807,18 @@
       <c r="F32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="G32" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H32" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+    </row>
+    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>44322</v>
       </c>
@@ -1699,16 +1838,16 @@
       <c r="F33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H33" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
+      <c r="H33" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
@@ -1730,18 +1869,18 @@
       <c r="F34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="G34" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H34" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+    </row>
+    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>44322</v>
       </c>
@@ -1761,16 +1900,18 @@
       <c r="F35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H35" s="20"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H35" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+    </row>
+    <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>44322</v>
       </c>
@@ -1790,14 +1931,16 @@
       <c r="F36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="G36" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H36" s="20"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
+      <c r="H36" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
@@ -1819,29 +1962,53 @@
       <c r="F37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="19" t="s">
+      <c r="G37" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H37" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="2"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
+      <c r="H37" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+    </row>
+    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>44322</v>
+      </c>
+      <c r="B38" s="9">
+        <v>1</v>
+      </c>
+      <c r="C38" s="10">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="3"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="K38" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L38" s="18"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
@@ -1849,12 +2016,12 @@
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="2"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
@@ -1862,12 +2029,12 @@
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="2"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
@@ -1875,12 +2042,12 @@
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="2"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E42" s="2"/>
@@ -2214,27 +2381,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"Implémentation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"Communication"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Organisation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Conception"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"Analyse"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Problème"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2243,8 +2410,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C1:D1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <color theme="5" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="82" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="48" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fin de Sprint 1
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Conception</t>
   </si>
   <si>
-    <t>Dossier de projet: Analyse / Conception: Concept</t>
-  </si>
-  <si>
     <t>Diagramme: Cas d'utilisation</t>
   </si>
   <si>
@@ -194,6 +191,21 @@
   </si>
   <si>
     <t>Dossier de projet: Stratégie de test</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Risques techniques</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Concept</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Analyse concurentielle</t>
+  </si>
+  <si>
+    <t>Base de données</t>
+  </si>
+  <si>
+    <t>Diagramme MCD</t>
   </si>
 </sst>
 </file>
@@ -373,13 +385,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -409,6 +414,13 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -696,11 +708,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L151"/>
+  <dimension ref="A1:L149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -746,7 +756,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L1" s="19" t="s">
         <v>8</v>
@@ -801,7 +811,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>12</v>
@@ -861,10 +871,10 @@
         <v>1.388888888888884E-2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>16</v>
@@ -1023,7 +1033,7 @@
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>44319</v>
       </c>
@@ -1047,7 +1057,7 @@
         <v>20</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
@@ -1078,7 +1088,7 @@
         <v>20</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
@@ -1109,7 +1119,7 @@
         <v>20</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
@@ -1140,7 +1150,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
@@ -1165,13 +1175,13 @@
         <v>1.3888888888888951E-2</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
@@ -1196,13 +1206,13 @@
         <v>1.7361111111111105E-2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
@@ -1227,13 +1237,13 @@
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="18" t="s">
         <v>31</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>32</v>
       </c>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
@@ -1261,10 +1271,10 @@
         <v>9</v>
       </c>
       <c r="G18" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="18" t="s">
         <v>33</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>34</v>
       </c>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
@@ -1292,7 +1302,7 @@
         <v>23</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
@@ -1318,13 +1328,13 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
@@ -1352,7 +1362,7 @@
         <v>23</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
@@ -1381,10 +1391,10 @@
         <v>9</v>
       </c>
       <c r="G22" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>40</v>
       </c>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
@@ -1412,12 +1422,12 @@
         <v>6</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
@@ -1440,13 +1450,13 @@
         <v>6.9444444444445308E-3</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
@@ -1467,17 +1477,17 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" ref="E25:E39" si="3">D25-C25</f>
+        <f t="shared" ref="E25:F44" si="3">D25-C25</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="18" t="s">
         <v>44</v>
-      </c>
-      <c r="H25" s="18" t="s">
-        <v>45</v>
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
@@ -1505,7 +1515,7 @@
         <v>23</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
@@ -1534,7 +1544,7 @@
         <v>23</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
@@ -1560,13 +1570,13 @@
         <v>1.2500000000000067E-2</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G28" s="15" t="s">
         <v>20</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
@@ -1597,7 +1607,7 @@
         <v>20</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
@@ -1625,7 +1635,7 @@
         <v>23</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="18"/>
@@ -1657,7 +1667,7 @@
         <v>20</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I31" s="18"/>
       <c r="J31" s="18"/>
@@ -1688,7 +1698,7 @@
         <v>20</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
@@ -1719,7 +1729,7 @@
         <v>20</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
@@ -1747,10 +1757,10 @@
         <v>9</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
@@ -1781,7 +1791,7 @@
         <v>20</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I35" s="18"/>
       <c r="J35" s="18"/>
@@ -1806,13 +1816,13 @@
         <v>3.125E-2</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
@@ -1843,7 +1853,7 @@
         <v>20</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
@@ -1874,16 +1884,16 @@
         <v>20</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I38" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="K38" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="J38" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="K38" s="18" t="s">
-        <v>56</v>
       </c>
       <c r="L38" s="18"/>
     </row>
@@ -1911,7 +1921,7 @@
         <v>20</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
@@ -1928,8 +1938,13 @@
       <c r="C40" s="10">
         <v>0.34375</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="2"/>
+      <c r="D40" s="10">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="3"/>
+        <v>5.555555555555558E-2</v>
+      </c>
       <c r="F40" s="1" t="s">
         <v>14</v>
       </c>
@@ -1937,7 +1952,7 @@
         <v>20</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
@@ -1945,82 +1960,134 @@
       <c r="L40" s="18"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="2"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="18"/>
+      <c r="A41" s="8">
+        <v>44323</v>
+      </c>
+      <c r="B41" s="9">
+        <v>1</v>
+      </c>
+      <c r="C41" s="10">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="2"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="18"/>
+      <c r="A42" s="8">
+        <v>44323</v>
+      </c>
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="10">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D42" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="3"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>57</v>
+      </c>
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="18"/>
       <c r="L42" s="18"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="2"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="18"/>
+      <c r="A43" s="8">
+        <v>44323</v>
+      </c>
+      <c r="B43" s="9">
+        <v>1</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0.46249999999999997</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1527777777777701E-2</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>59</v>
+      </c>
       <c r="I43" s="18"/>
       <c r="J43" s="18"/>
       <c r="K43" s="18"/>
       <c r="L43" s="18"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="2"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="18"/>
+      <c r="A44" s="8">
+        <v>44323</v>
+      </c>
+      <c r="B44" s="9">
+        <v>1</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0.46249999999999997</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0138888888888928E-2</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="I44" s="18"/>
       <c r="J44" s="18"/>
       <c r="K44" s="18"/>
       <c r="L44" s="18"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
       <c r="E45" s="2"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
       <c r="E46" s="2"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E47" s="2"/>
@@ -2331,31 +2398,25 @@
     <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" s="2"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E150" s="2"/>
-    </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E151" s="2"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"Problème"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Implémentation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Communication"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Organisation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>"Conception"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>"Analyse"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"Problème"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
@@ -2394,5 +2455,6 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalisation de la conception
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="76">
   <si>
     <t>Date</t>
   </si>
@@ -209,6 +209,45 @@
   </si>
   <si>
     <t>La conception des Wireframes m'aura demandé beaucoup de temps.</t>
+  </si>
+  <si>
+    <t>Rédaction d'un email.</t>
+  </si>
+  <si>
+    <t>Réponse au mail du Chef de projet pour le déplacement de la sprint review.</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Budget initial</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Planification détaillée</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Historique</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Analyse de l'environnement</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Charte graphique</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Conception de la base de données</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Conception du code</t>
+  </si>
+  <si>
+    <t>La conception du code étant normalisée en modèle MVC, les diagrammes de flux de la partie "Conception du code" du dossier de projet sont abandonnés.</t>
+  </si>
+  <si>
+    <t>Dossier de projet: Finalisation de la conception</t>
+  </si>
+  <si>
+    <t>Réalisation</t>
+  </si>
+  <si>
+    <t>Mise en place</t>
   </si>
 </sst>
 </file>
@@ -323,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -377,14 +416,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -417,6 +453,48 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -713,8 +791,8 @@
   </sheetPr>
   <dimension ref="A1:L149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,16 +832,16 @@
       <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1482,7 +1560,7 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" ref="E25:E45" si="3">D25-C25</f>
+        <f t="shared" ref="E25:E55" si="3">D25-C25</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -2121,7 +2199,7 @@
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>44326</v>
       </c>
@@ -2131,149 +2209,396 @@
       <c r="C46" s="10">
         <v>0.38263888888888892</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="2"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="18"/>
+      <c r="D46" s="10">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" si="3"/>
+        <v>4.8611111111110938E-3</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>64</v>
+      </c>
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
       <c r="K46" s="18"/>
       <c r="L46" s="18"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="2"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="18"/>
+      <c r="A47" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B47" s="9">
+        <v>2</v>
+      </c>
+      <c r="C47" s="10">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="D47" s="10">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" si="3"/>
+        <v>1.1805555555555569E-2</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>65</v>
+      </c>
       <c r="I47" s="18"/>
       <c r="J47" s="18"/>
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="2"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="18"/>
+      <c r="A48" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B48" s="9">
+        <v>2</v>
+      </c>
+      <c r="C48" s="10">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D48" s="10">
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="3"/>
+        <v>3.333333333333327E-2</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="I48" s="18"/>
       <c r="J48" s="18"/>
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="2"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="18"/>
+      <c r="A49" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B49" s="9">
+        <v>2</v>
+      </c>
+      <c r="C49" s="10">
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="D49" s="10">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5277777777777779E-2</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="I49" s="18"/>
       <c r="J49" s="18"/>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="2"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="18"/>
+      <c r="A50" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B50" s="9">
+        <v>2</v>
+      </c>
+      <c r="C50" s="10">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D50" s="10">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="3"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>67</v>
+      </c>
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="2"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="18"/>
+    <row r="51" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B51" s="9">
+        <v>2</v>
+      </c>
+      <c r="C51" s="10">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="D51" s="10">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>68</v>
+      </c>
       <c r="I51" s="18"/>
       <c r="J51" s="18"/>
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="2"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="18"/>
+      <c r="A52" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B52" s="9">
+        <v>2</v>
+      </c>
+      <c r="C52" s="10">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="D52" s="10">
+        <v>0.47986111111111113</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" si="3"/>
+        <v>4.1666666666667074E-3</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>69</v>
+      </c>
       <c r="I52" s="18"/>
       <c r="J52" s="18"/>
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="2"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="18"/>
+    <row r="53" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B53" s="9">
+        <v>2</v>
+      </c>
+      <c r="C53" s="10">
+        <v>0.47986111111111113</v>
+      </c>
+      <c r="D53" s="10">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="3"/>
+        <v>3.0555555555555503E-2</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>70</v>
+      </c>
       <c r="I53" s="18"/>
       <c r="J53" s="18"/>
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="2"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="18"/>
+    <row r="54" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B54" s="9">
+        <v>2</v>
+      </c>
+      <c r="C54" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="D54" s="10">
+        <v>0.59305555555555556</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="3"/>
+        <v>3.0555555555555558E-2</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>71</v>
+      </c>
       <c r="I54" s="18"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="2"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="18"/>
+      <c r="L54" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B55" s="9">
+        <v>2</v>
+      </c>
+      <c r="C55" s="10">
+        <v>0.59305555555555556</v>
+      </c>
+      <c r="D55" s="10">
+        <v>0.60625000000000007</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="3"/>
+        <v>1.3194444444444509E-2</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" s="18" t="s">
+        <v>73</v>
+      </c>
       <c r="I55" s="18"/>
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B56" s="9">
+        <v>2</v>
+      </c>
+      <c r="C56" s="10">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="D56" s="10"/>
       <c r="E56" s="2"/>
+      <c r="F56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G56" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
       <c r="E57" s="2"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
       <c r="E58" s="2"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
       <c r="E59" s="2"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="8"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
       <c r="E60" s="2"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="18"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
       <c r="E61" s="2"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E62" s="2"/>
@@ -2541,27 +2866,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"Problème"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"Implémentation"</formula>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"Réalisation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"Communication"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Organisation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Conception"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"Analyse"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2571,12 +2896,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color theme="4" tint="0.59999389629810485"/>
         <color theme="5" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="0" tint="-0.34998626667073579"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Base du site web
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -247,7 +247,16 @@
     <t>Réalisation</t>
   </si>
   <si>
-    <t>Mise en place</t>
+    <t>Implémentation de la base mvc du site web.</t>
+  </si>
+  <si>
+    <t>Enivronnement</t>
+  </si>
+  <si>
+    <t>Implémentation</t>
+  </si>
+  <si>
+    <t>Mise en place du lien entre le site et la base de données.</t>
   </si>
 </sst>
 </file>
@@ -420,7 +429,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -453,48 +462,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -792,7 +759,7 @@
   <dimension ref="A1:L149"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +771,8 @@
     <col min="5" max="5" width="7.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="40.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" style="3" customWidth="1"/>
+    <col min="9" max="12" width="40.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1560,7 +1528,7 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" ref="E25:E55" si="3">D25-C25</f>
+        <f t="shared" ref="E25:E57" si="3">D25-C25</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -2521,41 +2489,79 @@
       <c r="C56" s="10">
         <v>0.6069444444444444</v>
       </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="2"/>
+      <c r="D56" s="10">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1527777777777812E-2</v>
+      </c>
       <c r="F56" s="1" t="s">
         <v>74</v>
       </c>
       <c r="G56" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H56" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="H56" s="18"/>
       <c r="I56" s="18"/>
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="2"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="18"/>
+      <c r="A57" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B57" s="9">
+        <v>2</v>
+      </c>
+      <c r="C57" s="10">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D57" s="10">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="3"/>
+        <v>5.0694444444444375E-2</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H57" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="I57" s="18"/>
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="8"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="10"/>
+    <row r="58" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B58" s="9">
+        <v>2</v>
+      </c>
+      <c r="C58" s="10">
+        <v>0.68958333333333333</v>
+      </c>
       <c r="D58" s="10"/>
       <c r="E58" s="2"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="18"/>
+      <c r="F58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>78</v>
+      </c>
       <c r="I58" s="18"/>
       <c r="J58" s="18"/>
       <c r="K58" s="18"/>
@@ -2866,22 +2872,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Problème"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Réalisation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"Communication"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"Organisation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"Conception"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"Analyse"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fin de journée 11.05.21
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -263,6 +263,36 @@
   </si>
   <si>
     <t>Recherche du problème.</t>
+  </si>
+  <si>
+    <t>Environnement</t>
+  </si>
+  <si>
+    <t>Installation du serveur MySQL.</t>
+  </si>
+  <si>
+    <t>Sprint Review</t>
+  </si>
+  <si>
+    <t>Review Scénarios</t>
+  </si>
+  <si>
+    <t>Review et corrections des scénarios.</t>
+  </si>
+  <si>
+    <t>Review MCD MLD</t>
+  </si>
+  <si>
+    <t>Review et corrections des diagrammes MCD et MLD.</t>
+  </si>
+  <si>
+    <t>Corrections de certains détails.</t>
+  </si>
+  <si>
+    <t>Mise en place de la base de données.</t>
+  </si>
+  <si>
+    <t>Création du script de création de la base de données.</t>
   </si>
 </sst>
 </file>
@@ -764,9 +794,7 @@
   </sheetPr>
   <dimension ref="A1:L149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1534,7 +1562,7 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" ref="E25:E58" si="3">D25-C25</f>
+        <f t="shared" ref="E25:E68" si="3">D25-C25</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -2583,99 +2611,377 @@
       <c r="L58" s="18"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="8"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="2"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="18"/>
+      <c r="A59" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B59" s="9">
+        <v>2</v>
+      </c>
+      <c r="C59" s="10">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D59" s="10">
+        <v>0.36388888888888887</v>
+      </c>
+      <c r="E59" s="2">
+        <f t="shared" si="3"/>
+        <v>3.0555555555555558E-2</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="I59" s="18"/>
       <c r="J59" s="18"/>
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="2"/>
-      <c r="G60" s="17"/>
+      <c r="A60" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B60" s="9">
+        <v>2</v>
+      </c>
+      <c r="C60" s="10">
+        <v>0.36388888888888887</v>
+      </c>
+      <c r="D60" s="10">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E60" s="2">
+        <f t="shared" si="3"/>
+        <v>3.5416666666666707E-2</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="H60" s="18"/>
       <c r="I60" s="18"/>
       <c r="J60" s="18"/>
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="2"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="18"/>
+    <row r="61" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B61" s="9">
+        <v>2</v>
+      </c>
+      <c r="C61" s="10">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="D61" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E61" s="2">
+        <f t="shared" si="3"/>
+        <v>2.7777777777777846E-2</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="I61" s="18"/>
       <c r="J61" s="18"/>
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E62" s="2"/>
+      <c r="A62" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B62" s="9">
+        <v>2</v>
+      </c>
+      <c r="C62" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="D62" s="10">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E62" s="2">
+        <f t="shared" si="3"/>
+        <v>6.9444444444444364E-2</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E63" s="2"/>
+      <c r="A63" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B63" s="9">
+        <v>2</v>
+      </c>
+      <c r="C63" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="D63" s="10">
+        <v>0.59375</v>
+      </c>
+      <c r="E63" s="2">
+        <f t="shared" si="3"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="18"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E68" s="2"/>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B64" s="9">
+        <v>2</v>
+      </c>
+      <c r="C64" s="10">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D64" s="10">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="E64" s="2">
+        <f t="shared" si="3"/>
+        <v>9.7222222222221877E-3</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="18"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B65" s="9">
+        <v>2</v>
+      </c>
+      <c r="C65" s="10">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="D65" s="10">
+        <v>0.62083333333333335</v>
+      </c>
+      <c r="E65" s="2">
+        <f t="shared" si="3"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B66" s="9">
+        <v>2</v>
+      </c>
+      <c r="C66" s="10">
+        <v>0.62083333333333335</v>
+      </c>
+      <c r="D66" s="10">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E66" s="2">
+        <f t="shared" si="3"/>
+        <v>7.6388888888888618E-3</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H66" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B67" s="9">
+        <v>2</v>
+      </c>
+      <c r="C67" s="10">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D67" s="10">
+        <v>0.65902777777777777</v>
+      </c>
+      <c r="E67" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0138888888888817E-2</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H67" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
+    </row>
+    <row r="68" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B68" s="9">
+        <v>2</v>
+      </c>
+      <c r="C68" s="10">
+        <v>0.65902777777777777</v>
+      </c>
+      <c r="D68" s="10">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="E68" s="2">
+        <f t="shared" si="3"/>
+        <v>1.1111111111111072E-2</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G68" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H68" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="18"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
       <c r="E69" s="2"/>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="G69" s="17"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="18"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="8"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
       <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="G70" s="17"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+      <c r="J70" s="18"/>
+      <c r="K70" s="18"/>
+      <c r="L70" s="18"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
       <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="G71" s="17"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
+      <c r="J71" s="18"/>
+      <c r="K71" s="18"/>
+      <c r="L71" s="18"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E73" s="2"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E74" s="2"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E77" s="2"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E80" s="2"/>
     </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.25">
@@ -2946,7 +3252,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add article; Add artwork
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="141">
   <si>
     <t>Date</t>
   </si>
@@ -432,6 +432,28 @@
   </si>
   <si>
     <t>Notation des articles</t>
+  </si>
+  <si>
+    <t>Correstions en fonction de la sprint review: date, historique, MCD, stratégire de test.</t>
+  </si>
+  <si>
+    <t>Création d'article</t>
+  </si>
+  <si>
+    <t>Gestion des œuvres</t>
+  </si>
+  <si>
+    <t>Création d'œuvre</t>
+  </si>
+  <si>
+    <t>Modification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.php.net/manual/fr/reserved.variables.files.php
+https://www.php.net/manual/fr/function.strlen.php
+https://www.php.net/manual/fr/function.str-contains.php
+https://www.php.net/manual/fr/language.operators.comparison.php
+</t>
   </si>
 </sst>
 </file>
@@ -936,8 +958,8 @@
   </sheetPr>
   <dimension ref="A1:L149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G121" sqref="G121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4169,15 +4191,28 @@
       <c r="L104" s="13"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A105" s="6"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
+      <c r="A105" s="6">
+        <v>44341</v>
+      </c>
+      <c r="B105" s="7">
+        <v>4</v>
+      </c>
+      <c r="C105" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D105" s="8">
+        <v>0.36805555555555558</v>
+      </c>
       <c r="E105" s="2">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G105" s="18"/>
+        <v>3.4722222222222265E-2</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G105" s="18" t="s">
+        <v>134</v>
+      </c>
       <c r="H105" s="13"/>
       <c r="I105" s="13"/>
       <c r="J105" s="13"/>
@@ -4185,98 +4220,340 @@
       <c r="L105" s="13"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A106" s="6"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
+      <c r="A106" s="6">
+        <v>44341</v>
+      </c>
+      <c r="B106" s="7">
+        <v>4</v>
+      </c>
+      <c r="C106" s="8">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D106" s="8">
+        <v>0.3923611111111111</v>
+      </c>
       <c r="E106" s="2">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G106" s="18"/>
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G106" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="H106" s="13"/>
       <c r="I106" s="13"/>
       <c r="J106" s="13"/>
       <c r="K106" s="13"/>
       <c r="L106" s="13"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A107" s="6"/>
-      <c r="B107" s="7"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
+    <row r="107" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="6">
+        <v>44341</v>
+      </c>
+      <c r="B107" s="7">
+        <v>4</v>
+      </c>
+      <c r="C107" s="8">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D107" s="8">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E107" s="2">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G107" s="18"/>
-      <c r="H107" s="13"/>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G107" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H107" s="13" t="s">
+        <v>135</v>
+      </c>
       <c r="I107" s="13"/>
       <c r="J107" s="13"/>
       <c r="K107" s="13"/>
       <c r="L107" s="13"/>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E108" s="2"/>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E109" s="2"/>
+      <c r="A108" s="6">
+        <v>44341</v>
+      </c>
+      <c r="B108" s="7">
+        <v>4</v>
+      </c>
+      <c r="C108" s="8">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D108" s="8">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E108" s="2">
+        <f t="shared" ref="E108:E117" si="8">D108-C108</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G108" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="H108" s="13"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="13"/>
+      <c r="K108" s="13"/>
+      <c r="L108" s="13"/>
+    </row>
+    <row r="109" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A109" s="6">
+        <v>44341</v>
+      </c>
+      <c r="B109" s="7">
+        <v>4</v>
+      </c>
+      <c r="C109" s="8">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="D109" s="8">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="E109" s="2">
+        <f t="shared" si="8"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G109" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H109" s="13"/>
+      <c r="I109" s="13"/>
+      <c r="J109" s="13"/>
+      <c r="K109" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="L109" s="13"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E110" s="2"/>
+      <c r="A110" s="6">
+        <v>44341</v>
+      </c>
+      <c r="B110" s="7">
+        <v>4</v>
+      </c>
+      <c r="C110" s="8">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D110" s="8">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E110" s="2">
+        <f t="shared" si="8"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G110" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H110" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="I110" s="13"/>
+      <c r="J110" s="13"/>
+      <c r="K110" s="13"/>
+      <c r="L110" s="13"/>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E111" s="2"/>
+      <c r="A111" s="6">
+        <v>44341</v>
+      </c>
+      <c r="B111" s="7">
+        <v>4</v>
+      </c>
+      <c r="C111" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="D111" s="8">
+        <v>0.59375</v>
+      </c>
+      <c r="E111" s="2">
+        <f t="shared" si="8"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G111" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H111" s="13"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="13"/>
+      <c r="K111" s="13"/>
+      <c r="L111" s="13"/>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E112" s="2"/>
-    </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E113" s="2"/>
-    </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E114" s="2"/>
-    </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E115" s="2"/>
-    </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E116" s="2"/>
-    </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E117" s="2"/>
-    </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="6">
+        <v>44341</v>
+      </c>
+      <c r="B112" s="7">
+        <v>4</v>
+      </c>
+      <c r="C112" s="8">
+        <v>0.59375</v>
+      </c>
+      <c r="D112" s="8">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="E112" s="2">
+        <f t="shared" si="8"/>
+        <v>1.3194444444444398E-2</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G112" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H112" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="I112" s="13"/>
+      <c r="J112" s="13"/>
+      <c r="K112" s="13"/>
+      <c r="L112" s="13"/>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" s="6">
+        <v>44341</v>
+      </c>
+      <c r="B113" s="7">
+        <v>4</v>
+      </c>
+      <c r="C113" s="8">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="D113" s="8"/>
+      <c r="E113" s="2">
+        <f t="shared" si="8"/>
+        <v>-0.6069444444444444</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G113" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H113" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="I113" s="13"/>
+      <c r="J113" s="13"/>
+      <c r="K113" s="13"/>
+      <c r="L113" s="13"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" s="6"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G114" s="18"/>
+      <c r="H114" s="13"/>
+      <c r="I114" s="13"/>
+      <c r="J114" s="13"/>
+      <c r="K114" s="13"/>
+      <c r="L114" s="13"/>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A115" s="6"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="8"/>
+      <c r="D115" s="8"/>
+      <c r="E115" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G115" s="18"/>
+      <c r="H115" s="13"/>
+      <c r="I115" s="13"/>
+      <c r="J115" s="13"/>
+      <c r="K115" s="13"/>
+      <c r="L115" s="13"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" s="6"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G116" s="18"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="13"/>
+      <c r="J116" s="13"/>
+      <c r="K116" s="13"/>
+      <c r="L116" s="13"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" s="6"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G117" s="18"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="13"/>
+      <c r="K117" s="13"/>
+      <c r="L117" s="13"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E118" s="2"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E119" s="2"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E120" s="2"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E121" s="2"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E122" s="2"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E123" s="2"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E124" s="2"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E125" s="2"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E126" s="2"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E127" s="2"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E128" s="2"/>
     </row>
     <row r="129" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gestion des articles et des œuvres
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="146">
   <si>
     <t>Date</t>
   </si>
@@ -454,6 +454,27 @@
 https://www.php.net/manual/fr/function.str-contains.php
 https://www.php.net/manual/fr/language.operators.comparison.php
 </t>
+  </si>
+  <si>
+    <t>Gestion des articles</t>
+  </si>
+  <si>
+    <t>Pop-up de confirmation</t>
+  </si>
+  <si>
+    <t>Suppression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tutorialrepublic.com/faq/how-to-get-the-current-url-with-javascript.php
+https://www.w3schools.com/howto/howto_js_redirect_webpage.asp
+https://www.w3schools.com/tags/att_script_src.asp
+https://www.w3schools.com/js/js_window_location.asp
+https://www.w3schools.com/howto/tryit.asp?filename=tryhow_js_redirect_webpage
+https://developer.mozilla.org/fr/docs/Web/API/window/location
+</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/sql/sql_delete.asp</t>
   </si>
 </sst>
 </file>
@@ -958,8 +979,8 @@
   </sheetPr>
   <dimension ref="A1:L149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G119" sqref="G119"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H122" sqref="H122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4462,89 +4483,253 @@
       <c r="L113" s="13"/>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" s="6"/>
-      <c r="B114" s="7"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="8"/>
+      <c r="A114" s="6">
+        <v>44343</v>
+      </c>
+      <c r="B114" s="7">
+        <v>4</v>
+      </c>
+      <c r="C114" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="D114" s="8">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="E114" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G114" s="18"/>
-      <c r="H114" s="13"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G114" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="H114" s="13" t="s">
+        <v>139</v>
+      </c>
       <c r="I114" s="13"/>
       <c r="J114" s="13"/>
       <c r="K114" s="13"/>
       <c r="L114" s="13"/>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A115" s="6"/>
-      <c r="B115" s="7"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
+      <c r="A115" s="6">
+        <v>44343</v>
+      </c>
+      <c r="B115" s="7">
+        <v>4</v>
+      </c>
+      <c r="C115" s="8">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="D115" s="8">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="E115" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G115" s="18"/>
-      <c r="H115" s="13"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G115" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H115" s="13" t="s">
+        <v>143</v>
+      </c>
       <c r="I115" s="13"/>
       <c r="J115" s="13"/>
-      <c r="K115" s="13"/>
+      <c r="K115" t="s">
+        <v>145</v>
+      </c>
       <c r="L115" s="13"/>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A116" s="6"/>
-      <c r="B116" s="7"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
+      <c r="A116" s="6">
+        <v>44343</v>
+      </c>
+      <c r="B116" s="7">
+        <v>4</v>
+      </c>
+      <c r="C116" s="8">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D116" s="8">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E116" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G116" s="18"/>
-      <c r="H116" s="13"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G116" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="H116" s="13" t="s">
+        <v>143</v>
+      </c>
       <c r="I116" s="13"/>
       <c r="J116" s="13"/>
       <c r="K116" s="13"/>
       <c r="L116" s="13"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A117" s="6"/>
-      <c r="B117" s="7"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="8"/>
+    <row r="117" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+      <c r="A117" s="6">
+        <v>44343</v>
+      </c>
+      <c r="B117" s="7">
+        <v>4</v>
+      </c>
+      <c r="C117" s="8">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D117" s="8">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="E117" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G117" s="18"/>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G117" s="18" t="s">
+        <v>142</v>
+      </c>
       <c r="H117" s="13"/>
       <c r="I117" s="13"/>
       <c r="J117" s="13"/>
-      <c r="K117" s="13"/>
+      <c r="K117" s="13" t="s">
+        <v>144</v>
+      </c>
       <c r="L117" s="13"/>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E118" s="2"/>
+      <c r="A118" s="6">
+        <v>44343</v>
+      </c>
+      <c r="B118" s="7">
+        <v>4</v>
+      </c>
+      <c r="C118" s="8">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D118" s="8"/>
+      <c r="E118" s="2">
+        <f t="shared" ref="E118:E124" si="9">D118-C118</f>
+        <v>-0.63888888888888895</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G118" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="H118" s="13"/>
+      <c r="I118" s="13"/>
+      <c r="J118" s="13"/>
+      <c r="K118" s="13"/>
+      <c r="L118" s="13"/>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E119" s="2"/>
+      <c r="A119" s="6"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="8"/>
+      <c r="D119" s="8"/>
+      <c r="E119" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G119" s="18"/>
+      <c r="H119" s="13"/>
+      <c r="I119" s="13"/>
+      <c r="J119" s="13"/>
+      <c r="K119" s="13"/>
+      <c r="L119" s="13"/>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E120" s="2"/>
+      <c r="A120" s="6"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G120" s="18"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="13"/>
+      <c r="J120" s="13"/>
+      <c r="K120" s="13"/>
+      <c r="L120" s="13"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E121" s="2"/>
+      <c r="A121" s="6"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G121" s="18"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="13"/>
+      <c r="J121" s="13"/>
+      <c r="K121" s="13"/>
+      <c r="L121" s="13"/>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E122" s="2"/>
+      <c r="A122" s="6"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G122" s="18"/>
+      <c r="H122" s="13"/>
+      <c r="I122" s="13"/>
+      <c r="J122" s="13"/>
+      <c r="K122" s="13"/>
+      <c r="L122" s="13"/>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E123" s="2"/>
+      <c r="A123" s="6"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G123" s="18"/>
+      <c r="H123" s="13"/>
+      <c r="I123" s="13"/>
+      <c r="J123" s="13"/>
+      <c r="K123" s="13"/>
+      <c r="L123" s="13"/>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E124" s="2"/>
+      <c r="A124" s="6"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G124" s="18"/>
+      <c r="H124" s="13"/>
+      <c r="I124" s="13"/>
+      <c r="J124" s="13"/>
+      <c r="K124" s="13"/>
+      <c r="L124" s="13"/>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E125" s="2"/>

</xml_diff>

<commit_message>
note moyenne des articles
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="166">
   <si>
     <t>Date</t>
   </si>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:L148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H138" sqref="H138"/>
+      <selection activeCell="G141" sqref="G141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5275,10 +5275,12 @@
       <c r="C138" s="8">
         <v>0.3743055555555555</v>
       </c>
-      <c r="D138" s="8"/>
+      <c r="D138" s="8">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E138" s="2">
         <f t="shared" si="12"/>
-        <v>-0.3743055555555555</v>
+        <v>2.5000000000000078E-2</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>74</v>
@@ -5293,15 +5295,28 @@
       <c r="L138" s="13"/>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A139" s="6"/>
-      <c r="B139" s="7"/>
-      <c r="C139" s="8"/>
-      <c r="D139" s="8"/>
+      <c r="A139" s="6">
+        <v>44348</v>
+      </c>
+      <c r="B139" s="7">
+        <v>5</v>
+      </c>
+      <c r="C139" s="8">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D139" s="8">
+        <v>0.42430555555555555</v>
+      </c>
       <c r="E139" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="G139" s="18"/>
+        <v>1.4583333333333282E-2</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G139" s="18" t="s">
+        <v>165</v>
+      </c>
       <c r="H139" s="13"/>
       <c r="I139" s="13"/>
       <c r="J139" s="13"/>
@@ -5309,29 +5324,53 @@
       <c r="L139" s="13"/>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A140" s="6"/>
-      <c r="B140" s="7"/>
-      <c r="C140" s="8"/>
-      <c r="D140" s="8"/>
+      <c r="A140" s="6">
+        <v>44348</v>
+      </c>
+      <c r="B140" s="7">
+        <v>5</v>
+      </c>
+      <c r="C140" s="8">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="D140" s="8">
+        <v>0.45624999999999999</v>
+      </c>
       <c r="E140" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="G140" s="18"/>
-      <c r="H140" s="13"/>
+        <v>3.1944444444444442E-2</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G140" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H140" s="13" t="s">
+        <v>161</v>
+      </c>
       <c r="I140" s="13"/>
       <c r="J140" s="13"/>
       <c r="K140" s="13"/>
       <c r="L140" s="13"/>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A141" s="6"/>
-      <c r="B141" s="7"/>
-      <c r="C141" s="8"/>
+      <c r="A141" s="6">
+        <v>44348</v>
+      </c>
+      <c r="B141" s="7">
+        <v>5</v>
+      </c>
+      <c r="C141" s="8">
+        <v>0.45624999999999999</v>
+      </c>
       <c r="D141" s="8"/>
       <c r="E141" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-0.45624999999999999</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="G141" s="18"/>
       <c r="H141" s="13"/>

</xml_diff>

<commit_message>
toutes les fonctionnalités sont implémentées
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="167">
   <si>
     <t>Date</t>
   </si>
@@ -540,6 +540,9 @@
   </si>
   <si>
     <t>Commentaires utilisateur</t>
+  </si>
+  <si>
+    <t>Style du site</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1048,7 @@
   <dimension ref="A1:L148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G141" sqref="G141"/>
+      <selection activeCell="D142" sqref="D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5364,15 +5367,19 @@
       <c r="C141" s="8">
         <v>0.45624999999999999</v>
       </c>
-      <c r="D141" s="8"/>
+      <c r="D141" s="8">
+        <v>0.49374999999999997</v>
+      </c>
       <c r="E141" s="2">
         <f t="shared" si="12"/>
-        <v>-0.45624999999999999</v>
+        <v>3.7499999999999978E-2</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G141" s="18"/>
+      <c r="G141" s="18" t="s">
+        <v>166</v>
+      </c>
       <c r="H141" s="13"/>
       <c r="I141" s="13"/>
       <c r="J141" s="13"/>
@@ -5380,13 +5387,22 @@
       <c r="L141" s="13"/>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A142" s="6"/>
-      <c r="B142" s="7"/>
-      <c r="C142" s="8"/>
+      <c r="A142" s="6">
+        <v>44348</v>
+      </c>
+      <c r="B142" s="7">
+        <v>5</v>
+      </c>
+      <c r="C142" s="8">
+        <v>0.49374999999999997</v>
+      </c>
       <c r="D142" s="8"/>
       <c r="E142" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-0.49374999999999997</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="G142" s="18"/>
       <c r="H142" s="13"/>

</xml_diff>

<commit_message>
Correction des dernières erreurs et doc
Correction des dernières erreurs de code et ajout du Manuel d'installation et du Résumé du rapport
</commit_message>
<xml_diff>
--- a/Documentation/Édition/journal de travail.xlsx
+++ b/Documentation/Édition/journal de travail.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="182">
   <si>
     <t>Date</t>
   </si>
@@ -575,6 +575,24 @@
   </si>
   <si>
     <t>Rédaction d'un mail</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Tests de la stratégie</t>
+  </si>
+  <si>
+    <t>Manuel d'installation</t>
+  </si>
+  <si>
+    <t>Sources, glossaire</t>
+  </si>
+  <si>
+    <t>Vérification de l'exhaustivité</t>
+  </si>
+  <si>
+    <t>Vérification de l'exhaustivité de la documentation.</t>
   </si>
 </sst>
 </file>
@@ -750,7 +768,70 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1077,10 +1158,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L154"/>
+  <dimension ref="A1:L161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G148" sqref="G148"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D154" sqref="D154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5610,18 +5691,27 @@
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="6">
-        <v>44348</v>
+        <v>44350</v>
       </c>
       <c r="B148" s="7">
         <v>5</v>
       </c>
-      <c r="C148" s="8"/>
-      <c r="D148" s="8"/>
+      <c r="C148" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D148" s="8">
+        <v>0.37847222222222227</v>
+      </c>
       <c r="E148" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="G148" s="18"/>
+        <v>4.5138888888888951E-2</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G148" s="18" t="s">
+        <v>178</v>
+      </c>
       <c r="H148" s="13"/>
       <c r="I148" s="13"/>
       <c r="J148" s="13"/>
@@ -5630,19 +5720,30 @@
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="6">
-        <v>44348</v>
+        <v>44350</v>
       </c>
       <c r="B149" s="7">
         <v>5</v>
       </c>
-      <c r="C149" s="8"/>
-      <c r="D149" s="8"/>
+      <c r="C149" s="8">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="D149" s="8">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E149" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="G149" s="18"/>
-      <c r="H149" s="13"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G149" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H149" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="I149" s="13"/>
       <c r="J149" s="13"/>
       <c r="K149" s="13"/>
@@ -5650,34 +5751,58 @@
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="6">
-        <v>44348</v>
+        <v>44350</v>
       </c>
       <c r="B150" s="7">
         <v>5</v>
       </c>
-      <c r="C150" s="8"/>
-      <c r="D150" s="8"/>
+      <c r="C150" s="8">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D150" s="8">
+        <v>0.4236111111111111</v>
+      </c>
       <c r="E150" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="G150" s="18"/>
-      <c r="H150" s="13"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G150" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H150" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="I150" s="13"/>
       <c r="J150" s="13"/>
       <c r="K150" s="13"/>
       <c r="L150" s="13"/>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A151" s="6"/>
-      <c r="B151" s="7"/>
-      <c r="C151" s="8"/>
-      <c r="D151" s="8"/>
+      <c r="A151" s="6">
+        <v>44350</v>
+      </c>
+      <c r="B151" s="7">
+        <v>5</v>
+      </c>
+      <c r="C151" s="8">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="D151" s="8">
+        <v>0.4861111111111111</v>
+      </c>
       <c r="E151" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="G151" s="18"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G151" s="18" t="s">
+        <v>177</v>
+      </c>
       <c r="H151" s="13"/>
       <c r="I151" s="13"/>
       <c r="J151" s="13"/>
@@ -5685,76 +5810,232 @@
       <c r="L151" s="13"/>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A152" s="6"/>
-      <c r="B152" s="7"/>
-      <c r="C152" s="8"/>
-      <c r="D152" s="8"/>
+      <c r="A152" s="6">
+        <v>44350</v>
+      </c>
+      <c r="B152" s="7">
+        <v>5</v>
+      </c>
+      <c r="C152" s="8">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D152" s="8">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E152" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="G152" s="18"/>
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G152" s="18" t="s">
+        <v>179</v>
+      </c>
       <c r="H152" s="13"/>
       <c r="I152" s="13"/>
       <c r="J152" s="13"/>
       <c r="K152" s="13"/>
       <c r="L152" s="13"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A153" s="6"/>
-      <c r="B153" s="7"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
+    <row r="153" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="6">
+        <v>44350</v>
+      </c>
+      <c r="B153" s="7">
+        <v>5</v>
+      </c>
+      <c r="C153" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="D153" s="8">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="E153" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="G153" s="18"/>
-      <c r="H153" s="13"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G153" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H153" s="13" t="s">
+        <v>181</v>
+      </c>
       <c r="I153" s="13"/>
       <c r="J153" s="13"/>
       <c r="K153" s="13"/>
       <c r="L153" s="13"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A154" s="6"/>
-      <c r="B154" s="7"/>
-      <c r="C154" s="8"/>
+    <row r="154" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="6">
+        <v>44350</v>
+      </c>
+      <c r="B154" s="7">
+        <v>5</v>
+      </c>
+      <c r="C154" s="8">
+        <v>0.63888888888888895</v>
+      </c>
       <c r="D154" s="8"/>
       <c r="E154" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="G154" s="18"/>
-      <c r="H154" s="13"/>
+        <v>-0.63888888888888895</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G154" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H154" s="13" t="s">
+        <v>181</v>
+      </c>
       <c r="I154" s="13"/>
       <c r="J154" s="13"/>
       <c r="K154" s="13"/>
       <c r="L154" s="13"/>
     </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A155" s="6"/>
+      <c r="B155" s="7"/>
+      <c r="C155" s="8"/>
+      <c r="D155" s="8"/>
+      <c r="E155" s="2">
+        <f t="shared" ref="E155:E161" si="14">D155-C155</f>
+        <v>0</v>
+      </c>
+      <c r="G155" s="18"/>
+      <c r="H155" s="13"/>
+      <c r="I155" s="13"/>
+      <c r="J155" s="13"/>
+      <c r="K155" s="13"/>
+      <c r="L155" s="13"/>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A156" s="6"/>
+      <c r="B156" s="7"/>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G156" s="18"/>
+      <c r="H156" s="13"/>
+      <c r="I156" s="13"/>
+      <c r="J156" s="13"/>
+      <c r="K156" s="13"/>
+      <c r="L156" s="13"/>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A157" s="6"/>
+      <c r="B157" s="7"/>
+      <c r="C157" s="8"/>
+      <c r="D157" s="8"/>
+      <c r="E157" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G157" s="18"/>
+      <c r="H157" s="13"/>
+      <c r="I157" s="13"/>
+      <c r="J157" s="13"/>
+      <c r="K157" s="13"/>
+      <c r="L157" s="13"/>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A158" s="6"/>
+      <c r="B158" s="7"/>
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G158" s="18"/>
+      <c r="H158" s="13"/>
+      <c r="I158" s="13"/>
+      <c r="J158" s="13"/>
+      <c r="K158" s="13"/>
+      <c r="L158" s="13"/>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A159" s="6"/>
+      <c r="B159" s="7"/>
+      <c r="C159" s="8"/>
+      <c r="D159" s="8"/>
+      <c r="E159" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G159" s="18"/>
+      <c r="H159" s="13"/>
+      <c r="I159" s="13"/>
+      <c r="J159" s="13"/>
+      <c r="K159" s="13"/>
+      <c r="L159" s="13"/>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A160" s="6"/>
+      <c r="B160" s="7"/>
+      <c r="C160" s="8"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G160" s="18"/>
+      <c r="H160" s="13"/>
+      <c r="I160" s="13"/>
+      <c r="J160" s="13"/>
+      <c r="K160" s="13"/>
+      <c r="L160" s="13"/>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A161" s="6"/>
+      <c r="B161" s="7"/>
+      <c r="C161" s="8"/>
+      <c r="D161" s="8"/>
+      <c r="E161" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G161" s="18"/>
+      <c r="H161" s="13"/>
+      <c r="I161" s="13"/>
+      <c r="J161" s="13"/>
+      <c r="K161" s="13"/>
+      <c r="L161" s="13"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+  <conditionalFormatting sqref="F1:F149 F151:F1048576">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Problème"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"Réalisation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"Communication"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"Organisation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
       <formula>"Conception"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>"Analyse"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>"Documentation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5764,7 +6045,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5774,13 +6055,41 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color theme="0" tint="-4.9989318521683403E-2"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F150">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"Documentation"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"Problème"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"Réalisation"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Communication"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"Organisation"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+      <formula>"Conception"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+      <formula>"Analyse"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Tests"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>